<commit_message>
updated the actual execution for sprint1 for the last day
</commit_message>
<xml_diff>
--- a/Sprint Backlog/Sprint1/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
+++ b/Sprint Backlog/Sprint1/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint1\Planning and Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint Backlog\Sprint1\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A8BA0-1AB3-4AFD-9985-8C036FAD3E0D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88BAC63-4CF1-4D9A-8609-175BE7322015}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Actual" sheetId="1" r:id="rId1"/>
     <sheet name="Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>User Stories</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>T33</t>
+  </si>
+  <si>
+    <t>T:3</t>
   </si>
 </sst>
 </file>
@@ -1375,6 +1378,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Actual Execution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Burndown Chart for Sprint 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1436,6 +1469,64 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Burndown!$B$3:$I$3</c:f>
@@ -1479,22 +1570,25 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,8 +1601,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1525,6 +1620,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1590,6 +1740,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Story</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Points</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2823,15 +3033,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3215,7 +3425,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3677,9 @@
       <c r="D11" s="2">
         <v>3</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="I11" s="2"/>
@@ -3485,7 +3697,9 @@
       <c r="D12" s="2">
         <v>3</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3503,7 +3717,9 @@
       <c r="D13" s="2">
         <v>3</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3923,7 +4139,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4034,22 +4250,25 @@
         <v>56</v>
       </c>
       <c r="C5">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F5">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G5">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H5">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="I5">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typos within the excel charts
</commit_message>
<xml_diff>
--- a/Sprint Backlog/Sprint1/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
+++ b/Sprint Backlog/Sprint1/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint Backlog\Sprint1\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88BAC63-4CF1-4D9A-8609-175BE7322015}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8D1A6F-8253-4E99-A15D-879A0324FF5C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>User Stories</t>
   </si>
@@ -77,21 +77,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>A  = ARNOB</t>
-  </si>
-  <si>
-    <t>V = VILI</t>
-  </si>
-  <si>
-    <t>J = JAMES</t>
-  </si>
-  <si>
-    <t>M = MICHAEL</t>
-  </si>
-  <si>
-    <t>T = TONY</t>
-  </si>
-  <si>
     <t>J:2</t>
   </si>
   <si>
@@ -164,30 +149,6 @@
     <t>28</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -233,25 +194,22 @@
     <t>Planned to finish</t>
   </si>
   <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>T33</t>
-  </si>
-  <si>
     <t>T:3</t>
+  </si>
+  <si>
+    <t>A  = ARNOB (Talukder)</t>
+  </si>
+  <si>
+    <t>V = VILI (Vilen Milner)</t>
+  </si>
+  <si>
+    <t>J = JAMES (Qi Hang Yang)</t>
+  </si>
+  <si>
+    <t>M = MICHAEL (Rossinski)</t>
+  </si>
+  <si>
+    <t>T = TONY (Tianyi Zeng)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -347,6 +305,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3088,8 +3049,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31CD5ED-DA30-4B5B-9C2E-BD07FBAC5C04}" name="Table1" displayName="Table1" ref="A1:K35" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23" totalsRowBorderDxfId="22">
-  <autoFilter ref="A1:K34" xr:uid="{4F9759AE-BCDD-4C93-BCA3-CA94BFA349CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31CD5ED-DA30-4B5B-9C2E-BD07FBAC5C04}" name="Table1" displayName="Table1" ref="A1:K22" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:K21" xr:uid="{4F9759AE-BCDD-4C93-BCA3-CA94BFA349CB}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{3ACA0BEF-0DA9-435F-A244-9672369B292D}" name="User Stories" dataDxfId="21" totalsRowDxfId="10"/>
     <tableColumn id="2" xr3:uid="{6DF7373E-780B-4E1C-BCF0-8615D6B337E5}" name="Tasks" dataDxfId="20" totalsRowDxfId="9"/>
@@ -3424,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDF196-0978-4E31-AD1C-547BFF446FB7}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,7 +3394,7 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3470,8 +3431,8 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
+      <c r="L1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3479,22 +3440,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" t="s">
-        <v>12</v>
+      <c r="L2" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3502,22 +3463,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>13</v>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3525,23 +3486,23 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" t="s">
-        <v>14</v>
+      <c r="L4" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3549,23 +3510,23 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" t="s">
-        <v>15</v>
+      <c r="L5" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3573,7 +3534,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -3584,16 +3545,17 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
@@ -3603,17 +3565,18 @@
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
@@ -3623,37 +3586,39 @@
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -3665,73 +3630,77 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
@@ -3742,15 +3711,16 @@
       <c r="H14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
@@ -3761,13 +3731,14 @@
       <c r="H15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
@@ -3778,13 +3749,14 @@
       <c r="H16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -3796,13 +3768,14 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
@@ -3812,13 +3785,14 @@
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
@@ -3830,13 +3804,14 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -3848,13 +3823,14 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -3866,49 +3842,43 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>8</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5">
+        <f>SUBTOTAL(109,Table1[Story Points])</f>
+        <v>56</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>8</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2">
-        <v>5</v>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="3">
+        <v>56</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>8</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
@@ -3916,17 +3886,11 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>8</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
@@ -3934,17 +3898,11 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>44</v>
-      </c>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2">
-        <v>3</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
@@ -3952,19 +3910,11 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>9</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
@@ -3972,19 +3922,11 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="2">
-        <v>2</v>
-      </c>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
@@ -3992,19 +3934,11 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="2">
-        <v>3</v>
-      </c>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
@@ -4012,107 +3946,55 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>9</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="3">
-        <v>3</v>
-      </c>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>9</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>9</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="3">
-        <v>4</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="2">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="5">
-        <f>SUBTOTAL(109,Table1[Story Points])</f>
-        <v>103</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="7"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="3">
-        <v>56</v>
-      </c>
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -4138,7 +4020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C753B29C-8070-48CF-BECE-85E4DF604635}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -4149,36 +4031,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>56</v>
@@ -4186,7 +4068,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4215,7 +4097,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>56</v>
@@ -4244,7 +4126,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>56</v>

</xml_diff>